<commit_message>
upload of age group definition file;closes #867
</commit_message>
<xml_diff>
--- a/owlcms/src/main/resources/agegroups/AgeGroups_Masters.xlsx
+++ b/owlcms/src/main/resources/agegroups/AgeGroups_Masters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lamyj\git\owlcms4\owlcms\src\main\resources\agegroups\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B9C411-76DA-42A1-B36C-1930D11F5B10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8E3DAE1-DCD6-4EDD-B4FE-701E9AB86A3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2130" yWindow="1500" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AgeGroups" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="60">
   <si>
     <t>code</t>
   </si>
@@ -132,27 +132,6 @@
     <t>#default bw categories</t>
   </si>
   <si>
-    <t>U10</t>
-  </si>
-  <si>
-    <t>U</t>
-  </si>
-  <si>
-    <t>U13</t>
-  </si>
-  <si>
-    <t>U15</t>
-  </si>
-  <si>
-    <t>U17</t>
-  </si>
-  <si>
-    <t>U20</t>
-  </si>
-  <si>
-    <t>O21</t>
-  </si>
-  <si>
     <t>W30</t>
   </si>
   <si>
@@ -192,13 +171,7 @@
     <t>W85</t>
   </si>
   <si>
-    <t>YTH</t>
-  </si>
-  <si>
     <t>IWF</t>
-  </si>
-  <si>
-    <t>JR</t>
   </si>
   <si>
     <t>SR</t>
@@ -567,10 +540,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z984"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -580,7 +553,7 @@
     <col min="3" max="26" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -617,7 +590,7 @@
       <c r="T1" s="4"/>
       <c r="U1" s="4"/>
     </row>
-    <row r="2" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>35</v>
       </c>
@@ -629,32 +602,50 @@
         <v>18</v>
       </c>
       <c r="E2" s="3">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="F2" s="3">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="G2" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
     </row>
-    <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>37</v>
       </c>
@@ -666,20 +657,16 @@
         <v>18</v>
       </c>
       <c r="E3" s="3">
-        <v>11</v>
+        <v>35</v>
       </c>
       <c r="F3" s="3">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="G3" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>19</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
       <c r="J3" s="1" t="s">
         <v>20</v>
       </c>
@@ -699,15 +686,21 @@
         <v>25</v>
       </c>
       <c r="P3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="Q3" s="1"/>
-      <c r="R3" s="1"/>
-      <c r="S3" s="1"/>
       <c r="T3" s="1"/>
       <c r="U3" s="1"/>
     </row>
-    <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>38</v>
       </c>
@@ -719,20 +712,16 @@
         <v>18</v>
       </c>
       <c r="E4" s="3">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="F4" s="3">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="G4" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>19</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
       <c r="J4" s="1" t="s">
         <v>20</v>
       </c>
@@ -755,14 +744,18 @@
         <v>26</v>
       </c>
       <c r="Q4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S4" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
     </row>
-    <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>39</v>
       </c>
@@ -774,18 +767,16 @@
         <v>18</v>
       </c>
       <c r="E5" s="3">
-        <v>16</v>
+        <v>45</v>
       </c>
       <c r="F5" s="3">
-        <v>17</v>
+        <v>49</v>
       </c>
       <c r="G5" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" s="1"/>
-      <c r="I5" s="1" t="s">
-        <v>19</v>
-      </c>
+      <c r="I5" s="1"/>
       <c r="J5" s="1" t="s">
         <v>20</v>
       </c>
@@ -811,13 +802,15 @@
         <v>27</v>
       </c>
       <c r="R5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="S5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="S5" s="1"/>
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
     </row>
-    <row r="6" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>40</v>
       </c>
@@ -829,13 +822,13 @@
         <v>18</v>
       </c>
       <c r="E6" s="3">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="F6" s="3">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="G6" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -872,7 +865,7 @@
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
     </row>
-    <row r="7" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>41</v>
       </c>
@@ -884,13 +877,13 @@
         <v>18</v>
       </c>
       <c r="E7" s="3">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="F7" s="3">
-        <v>999</v>
+        <v>59</v>
       </c>
       <c r="G7" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -927,22 +920,22 @@
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
     </row>
-    <row r="8" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>42</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E8" s="3">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="F8" s="3">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="G8" s="5" t="b">
         <v>1</v>
@@ -982,22 +975,22 @@
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
     </row>
-    <row r="9" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E9" s="3">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="F9" s="3">
-        <v>39</v>
+        <v>69</v>
       </c>
       <c r="G9" s="5" t="b">
         <v>1</v>
@@ -1037,22 +1030,22 @@
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
     </row>
-    <row r="10" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E10" s="3">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="F10" s="3">
-        <v>44</v>
+        <v>74</v>
       </c>
       <c r="G10" s="5" t="b">
         <v>1</v>
@@ -1092,22 +1085,22 @@
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
     </row>
-    <row r="11" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E11" s="3">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="F11" s="3">
-        <v>49</v>
+        <v>79</v>
       </c>
       <c r="G11" s="5" t="b">
         <v>1</v>
@@ -1147,22 +1140,22 @@
       <c r="T11" s="1"/>
       <c r="U11" s="1"/>
     </row>
-    <row r="12" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E12" s="3">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="F12" s="3">
-        <v>54</v>
+        <v>84</v>
       </c>
       <c r="G12" s="5" t="b">
         <v>1</v>
@@ -1202,80 +1195,85 @@
       <c r="T12" s="1"/>
       <c r="U12" s="1"/>
     </row>
-    <row r="13" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D13" s="1" t="s">
+    <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="3">
-        <v>55</v>
-      </c>
-      <c r="F13" s="3">
-        <v>59</v>
+      <c r="E13" s="7">
+        <v>85</v>
+      </c>
+      <c r="F13" s="7">
+        <v>999</v>
       </c>
       <c r="G13" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1" t="s">
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="K13" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="L13" s="1" t="s">
+      <c r="L13" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="M13" s="1" t="s">
+      <c r="M13" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="N13" s="1" t="s">
+      <c r="N13" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="O13" s="1" t="s">
+      <c r="O13" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="P13" s="1" t="s">
+      <c r="P13" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="Q13" s="1" t="s">
+      <c r="Q13" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="R13" s="1" t="s">
+      <c r="R13" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="S13" s="1" t="s">
+      <c r="S13" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="T13" s="1"/>
-      <c r="U13" s="1"/>
+      <c r="T13" s="6"/>
+      <c r="U13" s="6"/>
+      <c r="V13" s="8"/>
+      <c r="W13" s="8"/>
+      <c r="X13" s="8"/>
+      <c r="Y13" s="8"/>
+      <c r="Z13" s="8"/>
     </row>
-    <row r="14" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E14" s="3">
-        <v>60</v>
+        <v>15</v>
       </c>
       <c r="F14" s="3">
-        <v>64</v>
+        <v>999</v>
       </c>
       <c r="G14" s="5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -1312,28 +1310,32 @@
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
     </row>
-    <row r="15" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="D15" s="1" t="s">
         <v>18</v>
       </c>
       <c r="E15" s="3">
-        <v>65</v>
+        <v>0</v>
       </c>
       <c r="F15" s="3">
-        <v>69</v>
+        <v>999</v>
       </c>
       <c r="G15" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
+        <v>0</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="J15" s="1" t="s">
         <v>20</v>
       </c>
@@ -1367,458 +1369,449 @@
       <c r="T15" s="1"/>
       <c r="U15" s="1"/>
     </row>
-    <row r="16" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="E16" s="3">
-        <v>70</v>
+        <v>30</v>
       </c>
       <c r="F16" s="3">
-        <v>74</v>
+        <v>34</v>
       </c>
       <c r="G16" s="5" t="b">
         <v>1</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
-      <c r="J16" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
       <c r="L16" s="1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="M16" s="1" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="T16" s="1"/>
-      <c r="U16" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="T16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U16" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>52</v>
+        <v>2</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="E17" s="3">
-        <v>75</v>
+        <v>35</v>
       </c>
       <c r="F17" s="3">
-        <v>79</v>
+        <v>39</v>
       </c>
       <c r="G17" s="5" t="b">
         <v>1</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
-      <c r="J17" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
       <c r="L17" s="1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="M17" s="1" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="Q17" s="1" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="S17" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="T17" s="1"/>
-      <c r="U17" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="T17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U17" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>53</v>
+        <v>4</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="E18" s="3">
-        <v>80</v>
+        <v>40</v>
       </c>
       <c r="F18" s="3">
-        <v>84</v>
+        <v>44</v>
       </c>
       <c r="G18" s="5" t="b">
         <v>1</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
-      <c r="J18" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
       <c r="L18" s="1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="M18" s="1" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="Q18" s="1" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="R18" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="S18" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="T18" s="1"/>
-      <c r="U18" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="T18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U18" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E19" s="7">
-        <v>85</v>
-      </c>
-      <c r="F19" s="7">
-        <v>999</v>
+    <row r="19" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="3">
+        <v>45</v>
+      </c>
+      <c r="F19" s="3">
+        <v>49</v>
       </c>
       <c r="G19" s="5" t="b">
         <v>1</v>
       </c>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="K19" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="L19" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="M19" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="N19" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="O19" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="P19" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q19" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="R19" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="S19" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="T19" s="6"/>
-      <c r="U19" s="6"/>
-      <c r="V19" s="8"/>
-      <c r="W19" s="8"/>
-      <c r="X19" s="8"/>
-      <c r="Y19" s="8"/>
-      <c r="Z19" s="8"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="T19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U19" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="E20" s="3">
+        <v>50</v>
+      </c>
+      <c r="F20" s="3">
+        <v>54</v>
+      </c>
+      <c r="G20" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P20" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q20" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R20" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F20" s="3">
-        <v>17</v>
-      </c>
-      <c r="G20" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="L20" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M20" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N20" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="O20" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="P20" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q20" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="R20" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="S20" s="1"/>
-      <c r="T20" s="1"/>
-      <c r="U20" s="1"/>
+      <c r="S20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="T20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U20" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>57</v>
+        <v>7</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="E21" s="3">
-        <v>15</v>
+        <v>55</v>
       </c>
       <c r="F21" s="3">
-        <v>20</v>
+        <v>59</v>
       </c>
       <c r="G21" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
-      <c r="J21" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K21" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
       <c r="L21" s="1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="M21" s="1" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="Q21" s="1" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="R21" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="S21" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="T21" s="1"/>
-      <c r="U21" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="T21" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U21" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="E22" s="3">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="F22" s="3">
-        <v>999</v>
+        <v>64</v>
       </c>
       <c r="G22" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
-      <c r="J22" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>21</v>
-      </c>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
       <c r="L22" s="1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="M22" s="1" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="N22" s="1" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="P22" s="1" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="S22" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="T22" s="1"/>
-      <c r="U22" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="T22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U22" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="E23" s="3">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="F23" s="3">
-        <v>999</v>
+        <v>69</v>
       </c>
       <c r="G23" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H23" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K23" s="1" t="s">
-        <v>21</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
       <c r="L23" s="1" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="N23" s="1" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="P23" s="1" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="Q23" s="1" t="s">
-        <v>27</v>
+        <v>12</v>
       </c>
       <c r="R23" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="S23" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="T23" s="1"/>
-      <c r="U23" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="T23" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U23" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1" t="s">
@@ -1828,34 +1821,52 @@
         <v>3</v>
       </c>
       <c r="E24" s="3">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="F24" s="3">
-        <v>10</v>
+        <v>74</v>
       </c>
       <c r="G24" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>16</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
-      <c r="P24" s="1"/>
-      <c r="Q24" s="1"/>
-      <c r="R24" s="1"/>
-      <c r="S24" s="1"/>
-      <c r="T24" s="1"/>
-      <c r="U24" s="1"/>
+      <c r="L24" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q24" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S24" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="T24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U24" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1" t="s">
@@ -1865,26 +1876,18 @@
         <v>3</v>
       </c>
       <c r="E25" s="3">
-        <v>11</v>
+        <v>75</v>
       </c>
       <c r="F25" s="3">
-        <v>13</v>
+        <v>79</v>
       </c>
       <c r="G25" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H25" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>6</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
       <c r="L25" s="1" t="s">
         <v>7</v>
       </c>
@@ -1898,17 +1901,27 @@
         <v>10</v>
       </c>
       <c r="P25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q25" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="R25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S25" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="T25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U25" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="Q25" s="1"/>
-      <c r="R25" s="1"/>
-      <c r="S25" s="1"/>
-      <c r="T25" s="1"/>
-      <c r="U25" s="1"/>
     </row>
-    <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>38</v>
+        <v>58</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1" t="s">
@@ -1918,24 +1931,18 @@
         <v>3</v>
       </c>
       <c r="E26" s="3">
-        <v>14</v>
+        <v>80</v>
       </c>
       <c r="F26" s="3">
-        <v>15</v>
+        <v>84</v>
       </c>
       <c r="G26" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H26" s="1"/>
-      <c r="I26" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J26" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K26" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
       <c r="L26" s="1" t="s">
         <v>7</v>
       </c>
@@ -1955,14 +1962,21 @@
         <v>12</v>
       </c>
       <c r="R26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="S26" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="T26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U26" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="T26" s="1"/>
-      <c r="U26" s="1"/>
     </row>
-    <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1" t="s">
@@ -1972,22 +1986,18 @@
         <v>3</v>
       </c>
       <c r="E27" s="3">
-        <v>16</v>
+        <v>85</v>
       </c>
       <c r="F27" s="3">
-        <v>17</v>
+        <v>999</v>
       </c>
       <c r="G27" s="5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
-      <c r="J27" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K27" s="1" t="s">
-        <v>6</v>
-      </c>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
       <c r="L27" s="1" t="s">
         <v>7</v>
       </c>
@@ -2010,26 +2020,31 @@
         <v>13</v>
       </c>
       <c r="S27" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="T27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U27" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="U27" s="1"/>
     </row>
-    <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="D28" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E28" s="3">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="F28" s="3">
-        <v>20</v>
+        <v>999</v>
       </c>
       <c r="G28" s="5" t="b">
         <v>0</v>
@@ -2069,30 +2084,38 @@
         <v>16</v>
       </c>
     </row>
-    <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>41</v>
+        <v>50</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="D29" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E29" s="3">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="F29" s="3">
-        <v>99</v>
+        <v>999</v>
       </c>
       <c r="G29" s="5" t="b">
         <v>0</v>
       </c>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="1"/>
-      <c r="K29" s="1"/>
+      <c r="H29" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="L29" s="1" t="s">
         <v>7</v>
       </c>
@@ -2124,897 +2147,25 @@
         <v>16</v>
       </c>
     </row>
-    <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E30" s="3">
-        <v>30</v>
-      </c>
-      <c r="F30" s="3">
-        <v>34</v>
-      </c>
-      <c r="G30" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="H30" s="1"/>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1"/>
-      <c r="K30" s="1"/>
-      <c r="L30" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M30" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N30" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O30" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="P30" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q30" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R30" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="S30" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="T30" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="U30" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E31" s="3">
-        <v>35</v>
-      </c>
-      <c r="F31" s="3">
-        <v>39</v>
-      </c>
-      <c r="G31" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-      <c r="J31" s="1"/>
-      <c r="K31" s="1"/>
-      <c r="L31" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M31" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N31" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O31" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="P31" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q31" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R31" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="S31" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="T31" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="U31" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="32" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E32" s="3">
-        <v>40</v>
-      </c>
-      <c r="F32" s="3">
-        <v>44</v>
-      </c>
-      <c r="G32" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-      <c r="J32" s="1"/>
-      <c r="K32" s="1"/>
-      <c r="L32" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M32" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N32" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O32" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="P32" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q32" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R32" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="S32" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="T32" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="U32" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="33" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E33" s="3">
-        <v>45</v>
-      </c>
-      <c r="F33" s="3">
-        <v>49</v>
-      </c>
-      <c r="G33" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="H33" s="1"/>
-      <c r="I33" s="1"/>
-      <c r="J33" s="1"/>
-      <c r="K33" s="1"/>
-      <c r="L33" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M33" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N33" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O33" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="P33" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q33" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R33" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="S33" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="T33" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="U33" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="34" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E34" s="3">
-        <v>50</v>
-      </c>
-      <c r="F34" s="3">
-        <v>54</v>
-      </c>
-      <c r="G34" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-      <c r="J34" s="1"/>
-      <c r="K34" s="1"/>
-      <c r="L34" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M34" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N34" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O34" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="P34" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q34" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R34" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="S34" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="T34" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="U34" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="35" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E35" s="3">
-        <v>55</v>
-      </c>
-      <c r="F35" s="3">
-        <v>59</v>
-      </c>
-      <c r="G35" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="H35" s="1"/>
-      <c r="I35" s="1"/>
-      <c r="J35" s="1"/>
-      <c r="K35" s="1"/>
-      <c r="L35" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M35" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N35" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O35" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="P35" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q35" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R35" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="S35" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="T35" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="U35" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="36" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E36" s="3">
-        <v>60</v>
-      </c>
-      <c r="F36" s="3">
-        <v>64</v>
-      </c>
-      <c r="G36" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="H36" s="1"/>
-      <c r="I36" s="1"/>
-      <c r="J36" s="1"/>
-      <c r="K36" s="1"/>
-      <c r="L36" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M36" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N36" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O36" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="P36" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q36" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R36" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="S36" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="T36" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="U36" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="37" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E37" s="3">
-        <v>65</v>
-      </c>
-      <c r="F37" s="3">
-        <v>69</v>
-      </c>
-      <c r="G37" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="H37" s="1"/>
-      <c r="I37" s="1"/>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1"/>
-      <c r="L37" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M37" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N37" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O37" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="P37" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q37" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R37" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="S37" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="T37" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="U37" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="38" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E38" s="3">
-        <v>70</v>
-      </c>
-      <c r="F38" s="3">
-        <v>74</v>
-      </c>
-      <c r="G38" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="H38" s="1"/>
-      <c r="I38" s="1"/>
-      <c r="J38" s="1"/>
-      <c r="K38" s="1"/>
-      <c r="L38" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M38" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N38" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O38" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="P38" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q38" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R38" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="S38" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="T38" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="U38" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="39" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E39" s="3">
-        <v>75</v>
-      </c>
-      <c r="F39" s="3">
-        <v>79</v>
-      </c>
-      <c r="G39" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="H39" s="1"/>
-      <c r="I39" s="1"/>
-      <c r="J39" s="1"/>
-      <c r="K39" s="1"/>
-      <c r="L39" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M39" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N39" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O39" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="P39" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q39" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R39" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="S39" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="T39" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="U39" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="40" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E40" s="3">
-        <v>80</v>
-      </c>
-      <c r="F40" s="3">
-        <v>84</v>
-      </c>
-      <c r="G40" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="H40" s="1"/>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1"/>
-      <c r="K40" s="1"/>
-      <c r="L40" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M40" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N40" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O40" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="P40" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q40" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R40" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="S40" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="T40" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="U40" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="41" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E41" s="3">
-        <v>85</v>
-      </c>
-      <c r="F41" s="3">
-        <v>999</v>
-      </c>
-      <c r="G41" s="5" t="b">
-        <v>1</v>
-      </c>
-      <c r="H41" s="1"/>
-      <c r="I41" s="1"/>
-      <c r="J41" s="1"/>
-      <c r="K41" s="1"/>
-      <c r="L41" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M41" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N41" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O41" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="P41" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q41" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R41" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="S41" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="T41" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="U41" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="42" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E42" s="3">
-        <v>13</v>
-      </c>
-      <c r="F42" s="3">
-        <v>17</v>
-      </c>
-      <c r="G42" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H42" s="1"/>
-      <c r="I42" s="1"/>
-      <c r="J42" s="1"/>
-      <c r="K42" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L42" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M42" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N42" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O42" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="P42" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q42" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R42" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="S42" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="T42" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="U42" s="1"/>
-    </row>
-    <row r="43" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E43" s="3">
-        <v>15</v>
-      </c>
-      <c r="F43" s="3">
-        <v>20</v>
-      </c>
-      <c r="G43" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H43" s="1"/>
-      <c r="I43" s="1"/>
-      <c r="J43" s="1"/>
-      <c r="K43" s="1"/>
-      <c r="L43" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M43" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N43" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O43" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="P43" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q43" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R43" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="S43" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="T43" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="U43" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="44" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E44" s="3">
-        <v>15</v>
-      </c>
-      <c r="F44" s="3">
-        <v>999</v>
-      </c>
-      <c r="G44" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H44" s="1"/>
-      <c r="I44" s="1"/>
-      <c r="J44" s="1"/>
-      <c r="K44" s="1"/>
-      <c r="L44" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M44" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N44" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O44" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="P44" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q44" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R44" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="S44" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="T44" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="U44" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="45" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E45" s="3">
-        <v>0</v>
-      </c>
-      <c r="F45" s="3">
-        <v>999</v>
-      </c>
-      <c r="G45" s="5" t="b">
-        <v>0</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I45" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J45" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="K45" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L45" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M45" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N45" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O45" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="P45" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q45" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="R45" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="S45" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="T45" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="U45" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="46" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="30" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="31" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="32" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="35" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3951,22 +3102,6 @@
     <row r="982" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="983" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="984" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="985" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="986" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="987" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="988" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="989" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="990" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="991" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="992" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="H1:J1"/>

</xml_diff>